<commit_message>
Continuo corrigiendo la propuesta de articulo
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/todomundomx/Desktop/MiGithub/ProyectoCertificacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CD911EB-8890-3347-82F6-DDBD65FF1FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B917AE4D-7796-F84B-8DB3-82972FAB8A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="7900" windowWidth="28040" windowHeight="17440" xr2:uid="{5A3A1A73-B642-6D44-B565-802F0378ADD6}"/>
+    <workbookView xWindow="300" yWindow="11440" windowWidth="23220" windowHeight="16040" xr2:uid="{5A3A1A73-B642-6D44-B565-802F0378ADD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>ISET</t>
   </si>
@@ -92,13 +92,97 @@
   </si>
   <si>
     <t>CPYAU</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>GAM</t>
+  </si>
+  <si>
+    <t>IZT</t>
+  </si>
+  <si>
+    <t>PESCER</t>
+  </si>
+  <si>
+    <t>SLT</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>G13</t>
+  </si>
+  <si>
+    <t>G14</t>
+  </si>
+  <si>
+    <t>G15</t>
+  </si>
+  <si>
+    <t>G16</t>
+  </si>
+  <si>
+    <t>G17</t>
+  </si>
+  <si>
+    <t>G18</t>
+  </si>
+  <si>
+    <t>G19</t>
+  </si>
+  <si>
+    <t>G20</t>
+  </si>
+  <si>
+    <t>G21</t>
+  </si>
+  <si>
+    <t>G22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +193,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,9 +228,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,337 +546,765 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547BA8C3-A4BD-D445-A501-214AC98EF90A}">
-  <dimension ref="B2:F21"/>
+  <dimension ref="B2:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2">
         <v>74000</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <f>C2/$C$21</f>
         <v>6.0502398838353941E-2</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <f>C2/$C$21</f>
         <v>6.0502398838353941E-2</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
+        <v>134038</v>
+      </c>
+      <c r="K2" s="4">
+        <f>I2/$J$7*100</f>
+        <v>10.958946669588224</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
         <v>92300</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D20" si="0">C3/$C$21</f>
         <v>7.5464478551082015E-2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E20" si="1">C3/$C$21</f>
         <v>7.5464478551082015E-2</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>86983</v>
+      </c>
+      <c r="J3">
+        <f>I3+I2</f>
+        <v>221021</v>
+      </c>
+      <c r="K3" s="4">
+        <f t="shared" ref="K3:K7" si="2">I3/$J$7*100</f>
+        <v>7.1117299434547849</v>
+      </c>
+      <c r="L3" s="4">
+        <f>K3+K2</f>
+        <v>18.070676613043009</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4">
         <v>248506</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
         <v>0.20317850169897278</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <f t="shared" si="1"/>
         <v>0.20317850169897278</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <f>D4+D8</f>
         <v>0.39913268993665241</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4">
+        <v>250641</v>
+      </c>
+      <c r="J4">
+        <f>J3+I4</f>
+        <v>471662</v>
+      </c>
+      <c r="K4" s="4">
+        <f t="shared" si="2"/>
+        <v>20.492407766545771</v>
+      </c>
+      <c r="L4" s="4">
+        <f>L3+K4</f>
+        <v>38.56308437958878</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
         <v>3800</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>3.1068799403479053E-3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <f t="shared" si="1"/>
         <v>3.1068799403479053E-3</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5">
+        <v>134405</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J7" si="3">J4+I5</f>
+        <v>606067</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" si="2"/>
+        <v>10.98895258901211</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" ref="L5:L7" si="4">L4+K5</f>
+        <v>49.552036968600888</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
         <v>6693</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
         <v>5.4721966949338235E-3</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <f t="shared" si="1"/>
         <v>5.4721966949338235E-3</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6">
+        <v>23965</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>630032</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="2"/>
+        <v>1.9593783623799357</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="4"/>
+        <v>51.511415330980824</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
         <v>44869</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>3.6684893695650041E-2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <f t="shared" si="1"/>
         <v>3.6684893695650041E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7">
+        <v>593060</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>1223092</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="2"/>
+        <v>48.488584669019176</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8">
         <v>239670</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>0.1959541882376796</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <f t="shared" si="1"/>
         <v>0.1959541882376796</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9">
         <v>65268</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>5.3363115775428176E-2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <f t="shared" si="1"/>
         <v>5.3363115775428176E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10">
         <v>59221</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>4.8419088670353501E-2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <f t="shared" si="1"/>
         <v>4.8419088670353501E-2</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10">
+        <v>26173</v>
+      </c>
+      <c r="K10">
+        <f>I10/$J$31*100</f>
+        <v>2.2010283182774577</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11">
         <v>43049</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>3.5196861724220256E-2</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <f t="shared" si="1"/>
         <v>3.5196861724220256E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11">
+        <v>2927</v>
+      </c>
+      <c r="J11">
+        <f>I11+I10</f>
+        <v>29100</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11:K31" si="5">I11/$J$31*100</f>
+        <v>0.2461471702746387</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12">
         <v>38518</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>3.1492316195347529E-2</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <f t="shared" si="1"/>
         <v>3.1492316195347529E-2</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12">
+        <v>5109</v>
+      </c>
+      <c r="J12">
+        <f>J11+I12</f>
+        <v>34209</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="5"/>
+        <v>0.42964328422723919</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13">
         <v>29875</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>2.4425799531024649E-2</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <f t="shared" si="1"/>
         <v>2.4425799531024649E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13">
+        <v>10144</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ref="J13:J30" si="6">J12+I13</f>
+        <v>44353</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="5"/>
+        <v>0.8530635105110812</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14">
         <v>32898</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>2.6897404283569838E-2</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <f t="shared" si="1"/>
         <v>2.6897404283569838E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14">
+        <v>12565</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="6"/>
+        <v>56918</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="5"/>
+        <v>1.056658419713302</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15">
         <v>44456</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>3.6347224902133282E-2</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <f t="shared" si="1"/>
         <v>3.6347224902133282E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15">
+        <v>28147</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="6"/>
+        <v>85065</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="5"/>
+        <v>2.3670325936864556</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>13</v>
       </c>
       <c r="C16">
         <v>9361</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>7.6535534530517736E-3</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <f t="shared" si="1"/>
         <v>7.6535534530517736E-3</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16">
+        <v>41332</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="6"/>
+        <v>126397</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="5"/>
+        <v>3.4758301475201114</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17">
         <v>7644</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>6.2497342800051014E-3</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <f t="shared" si="1"/>
         <v>6.2497342800051014E-3</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17">
+        <v>56299</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="6"/>
+        <v>182696</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="5"/>
+        <v>4.7344856642609781</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18">
         <v>21436</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>1.7526073263499392E-2</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <f t="shared" si="1"/>
         <v>1.7526073263499392E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18">
+        <v>99032</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="6"/>
+        <v>281728</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="5"/>
+        <v>8.3281334358175663</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19">
         <v>154107</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>0.12599788078084068</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <f t="shared" si="1"/>
         <v>0.12599788078084068</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19">
+        <v>71193</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="6"/>
+        <v>352921</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="5"/>
+        <v>5.9870022184360616</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20">
         <v>7421</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>6.0674094835057382E-3</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <f t="shared" si="1"/>
         <v>6.0674094835057382E-3</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20">
+        <v>72554</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="6"/>
+        <v>425475</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="5"/>
+        <v>6.1014560273680001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C21">
         <f>SUM(C2:C20)</f>
         <v>1223092</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" ref="D21:E21" si="2">SUM(D2:D20)</f>
+        <f t="shared" ref="D21:E21" si="7">SUM(D2:D20)</f>
         <v>0.99999999999999989</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.99999999999999989</v>
       </c>
+      <c r="H21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21">
+        <v>3774</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="6"/>
+        <v>429249</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="5"/>
+        <v>0.31737595511325123</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22">
+        <v>69575</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="6"/>
+        <v>498824</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="5"/>
+        <v>5.850935897457461</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23">
+        <v>74449</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="6"/>
+        <v>573273</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="5"/>
+        <v>6.2608167679455331</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24">
+        <v>78721</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="6"/>
+        <v>651994</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="5"/>
+        <v>6.620072221110294</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25">
+        <v>80783</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="6"/>
+        <v>732777</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="5"/>
+        <v>6.7934768897492779</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26">
+        <v>81429</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="6"/>
+        <v>814206</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="5"/>
+        <v>6.847802503687582</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27">
+        <v>82974</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="6"/>
+        <v>897180</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="5"/>
+        <v>6.9777298621004</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>43</v>
+      </c>
+      <c r="I28">
+        <v>86330</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="6"/>
+        <v>983510</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="5"/>
+        <v>7.2599539493712184</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I29">
+        <v>44395</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="6"/>
+        <v>1027905</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="5"/>
+        <v>3.7334142891501823</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>45</v>
+      </c>
+      <c r="I30">
+        <v>122594</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="6"/>
+        <v>1150499</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="5"/>
+        <v>10.309588723146243</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31">
+        <v>38627</v>
+      </c>
+      <c r="J31">
+        <f t="shared" ref="J31" si="8">J30+I31</f>
+        <v>1189126</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="5"/>
+        <v>3.2483521510756641</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>